<commit_message>
Remove HTML tags while rendering topic description
</commit_message>
<xml_diff>
--- a/database/seeds/seed_files/product-management.xlsx
+++ b/database/seeds/seed_files/product-management.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Roles" sheetId="1" r:id="rId1"/>
@@ -45,9 +45,6 @@
     <t>User</t>
   </si>
   <si>
-    <t>super-admin</t>
-  </si>
-  <si>
     <t>Master's degree</t>
   </si>
   <si>
@@ -373,6 +370,9 @@
   </si>
   <si>
     <t>Lean.png</t>
+  </si>
+  <si>
+    <t>super_admin</t>
   </si>
 </sst>
 </file>
@@ -766,7 +766,7 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -838,7 +838,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -846,7 +846,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -854,7 +854,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>
@@ -866,8 +866,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -881,19 +881,19 @@
         <v>1</v>
       </c>
       <c r="B1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C1" t="s">
         <v>45</v>
       </c>
-      <c r="C1" t="s">
-        <v>46</v>
-      </c>
       <c r="D1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -901,16 +901,16 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C2" s="4" t="s">
         <v>47</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>48</v>
       </c>
       <c r="D2" s="4">
         <v>123456</v>
       </c>
       <c r="E2" t="s">
-        <v>5</v>
+        <v>114</v>
       </c>
       <c r="F2" t="b">
         <v>1</v>
@@ -921,10 +921,10 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
+        <v>48</v>
+      </c>
+      <c r="C3" s="4" t="s">
         <v>49</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>50</v>
       </c>
       <c r="D3" s="4">
         <v>123456</v>
@@ -941,10 +941,10 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
+        <v>50</v>
+      </c>
+      <c r="C4" s="4" t="s">
         <v>51</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>52</v>
       </c>
       <c r="D4" s="4">
         <v>123456</v>
@@ -961,10 +961,10 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
+        <v>52</v>
+      </c>
+      <c r="C5" s="4" t="s">
         <v>53</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>54</v>
       </c>
       <c r="D5" s="4">
         <v>123456</v>
@@ -981,10 +981,10 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
+        <v>54</v>
+      </c>
+      <c r="C6" s="4" t="s">
         <v>55</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>56</v>
       </c>
       <c r="D6" s="4">
         <v>123456</v>
@@ -1001,10 +1001,10 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
+        <v>56</v>
+      </c>
+      <c r="C7" s="4" t="s">
         <v>57</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>58</v>
       </c>
       <c r="D7" s="4">
         <v>123456</v>
@@ -1021,10 +1021,10 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D8" s="4">
         <v>123456</v>
@@ -1055,8 +1055,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="E26" sqref="E26"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1075,13 +1075,13 @@
         <v>2</v>
       </c>
       <c r="C1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -1089,7 +1089,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -1103,7 +1103,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C3">
         <v>1</v>
@@ -1117,7 +1117,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C4">
         <v>1</v>
@@ -1131,7 +1131,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C5">
         <v>1</v>
@@ -1145,7 +1145,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C6">
         <v>1</v>
@@ -1159,7 +1159,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C7">
         <v>1</v>
@@ -1173,7 +1173,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C8">
         <v>1</v>
@@ -1187,7 +1187,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C9">
         <v>1</v>
@@ -1201,7 +1201,7 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C10">
         <v>2</v>
@@ -1215,7 +1215,7 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C11">
         <v>2</v>
@@ -1229,7 +1229,7 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C12">
         <v>2</v>
@@ -1243,7 +1243,7 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C13">
         <v>2</v>
@@ -1257,7 +1257,7 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C14">
         <v>2</v>
@@ -1271,7 +1271,7 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C15">
         <v>2</v>
@@ -1285,7 +1285,7 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C16">
         <v>2</v>
@@ -1299,7 +1299,7 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C17">
         <v>2</v>
@@ -1313,7 +1313,7 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C18">
         <v>3</v>
@@ -1322,7 +1322,7 @@
         <v>1</v>
       </c>
       <c r="E18" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
@@ -1330,7 +1330,7 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C19">
         <v>3</v>
@@ -1339,7 +1339,7 @@
         <v>1</v>
       </c>
       <c r="E19" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
@@ -1347,7 +1347,7 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C20">
         <v>3</v>
@@ -1356,7 +1356,7 @@
         <v>1</v>
       </c>
       <c r="E20" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
@@ -1364,7 +1364,7 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C21">
         <v>3</v>
@@ -1373,7 +1373,7 @@
         <v>1</v>
       </c>
       <c r="E21" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
@@ -1381,7 +1381,7 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C22">
         <v>3</v>
@@ -1390,7 +1390,7 @@
         <v>1</v>
       </c>
       <c r="E22" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
@@ -1398,7 +1398,7 @@
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C23">
         <v>3</v>
@@ -1407,7 +1407,7 @@
         <v>1</v>
       </c>
       <c r="E23" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
@@ -1415,7 +1415,7 @@
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C24">
         <v>3</v>
@@ -1424,7 +1424,7 @@
         <v>1</v>
       </c>
       <c r="E24" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
@@ -1432,7 +1432,7 @@
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C25">
         <v>3</v>
@@ -1441,7 +1441,7 @@
         <v>1</v>
       </c>
       <c r="E25" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
@@ -1449,7 +1449,7 @@
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C26">
         <v>3</v>
@@ -1458,7 +1458,7 @@
         <v>1</v>
       </c>
       <c r="E26" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
@@ -1466,7 +1466,7 @@
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C27">
         <v>3</v>
@@ -1475,7 +1475,7 @@
         <v>1</v>
       </c>
       <c r="E27" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
@@ -1483,7 +1483,7 @@
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C28">
         <v>3</v>
@@ -1492,7 +1492,7 @@
         <v>1</v>
       </c>
       <c r="E28" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
@@ -1500,7 +1500,7 @@
         <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C29">
         <v>3</v>
@@ -1509,7 +1509,7 @@
         <v>1</v>
       </c>
       <c r="E29" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
@@ -1517,7 +1517,7 @@
         <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C30">
         <v>3</v>
@@ -1526,7 +1526,7 @@
         <v>1</v>
       </c>
       <c r="E30" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
@@ -1534,7 +1534,7 @@
         <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C31">
         <v>3</v>
@@ -1543,7 +1543,7 @@
         <v>1</v>
       </c>
       <c r="E31" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
@@ -1551,7 +1551,7 @@
         <v>31</v>
       </c>
       <c r="B32" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C32">
         <v>3</v>
@@ -1560,7 +1560,7 @@
         <v>1</v>
       </c>
       <c r="E32" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
@@ -1568,7 +1568,7 @@
         <v>32</v>
       </c>
       <c r="B33" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C33">
         <v>3</v>
@@ -1577,7 +1577,7 @@
         <v>1</v>
       </c>
       <c r="E33" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
@@ -1585,7 +1585,7 @@
         <v>33</v>
       </c>
       <c r="B34" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C34">
         <v>3</v>
@@ -1594,7 +1594,7 @@
         <v>1</v>
       </c>
       <c r="E34" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
@@ -1602,7 +1602,7 @@
         <v>34</v>
       </c>
       <c r="B35" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C35">
         <v>3</v>
@@ -1611,7 +1611,7 @@
         <v>1</v>
       </c>
       <c r="E35" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
@@ -1619,7 +1619,7 @@
         <v>35</v>
       </c>
       <c r="B36" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C36">
         <v>3</v>
@@ -1628,7 +1628,7 @@
         <v>1</v>
       </c>
       <c r="E36" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
@@ -1636,7 +1636,7 @@
         <v>36</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C37">
         <v>3</v>
@@ -1645,7 +1645,7 @@
         <v>1</v>
       </c>
       <c r="E37" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
@@ -1653,7 +1653,7 @@
         <v>37</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C38">
         <v>3</v>
@@ -1662,7 +1662,7 @@
         <v>1</v>
       </c>
       <c r="E38" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
   </sheetData>
@@ -1689,16 +1689,16 @@
         <v>1</v>
       </c>
       <c r="B1" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="D1" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="C1" s="5" t="s">
-        <v>92</v>
-      </c>
-      <c r="D1" s="5" t="s">
-        <v>66</v>
-      </c>
       <c r="E1" s="8" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1712,10 +1712,10 @@
         <v>1</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1729,10 +1729,10 @@
         <v>1</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1746,10 +1746,10 @@
         <v>1</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1763,10 +1763,10 @@
         <v>1</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1780,10 +1780,10 @@
         <v>1</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E6" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1797,10 +1797,10 @@
         <v>1</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E7" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1814,10 +1814,10 @@
         <v>1</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E8" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1831,10 +1831,10 @@
         <v>1</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E9" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1848,10 +1848,10 @@
         <v>1</v>
       </c>
       <c r="D10" s="7" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E10" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1865,10 +1865,10 @@
         <v>1</v>
       </c>
       <c r="D11" s="7" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E11" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1882,10 +1882,10 @@
         <v>1</v>
       </c>
       <c r="D12" s="7" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E12" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1899,10 +1899,10 @@
         <v>1</v>
       </c>
       <c r="D13" s="7" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E13" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1916,10 +1916,10 @@
         <v>1</v>
       </c>
       <c r="D14" s="7" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E14" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1933,10 +1933,10 @@
         <v>1</v>
       </c>
       <c r="D15" s="7" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E15" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1950,10 +1950,10 @@
         <v>1</v>
       </c>
       <c r="D16" s="7" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E16" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1967,10 +1967,10 @@
         <v>1</v>
       </c>
       <c r="D17" s="7" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E17" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1984,10 +1984,10 @@
         <v>1</v>
       </c>
       <c r="D18" s="7" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E18" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2001,10 +2001,10 @@
         <v>1</v>
       </c>
       <c r="D19" s="7" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E19" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
   </sheetData>

</xml_diff>